<commit_message>
Bigger is greater hackerrank challenge.
</commit_message>
<xml_diff>
--- a/ClassesTaken/edX/2015/OptionsMath/opthw.xlsx
+++ b/ClassesTaken/edX/2015/OptionsMath/opthw.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="8688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="8688" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wk0" sheetId="1" r:id="rId1"/>
+    <sheet name="wk04" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>val</t>
   </si>
@@ -36,6 +37,165 @@
   </si>
   <si>
     <t>fn(num)</t>
+  </si>
+  <si>
+    <t>1 Practice</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>coeff2_u</t>
+  </si>
+  <si>
+    <t>coeff1_u</t>
+  </si>
+  <si>
+    <t>coeff0_u</t>
+  </si>
+  <si>
+    <t>ncoeff1</t>
+  </si>
+  <si>
+    <t>ncoeff0</t>
+  </si>
+  <si>
+    <t>sqrt</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>u_plus</t>
+  </si>
+  <si>
+    <t>u_minus</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>1 Real</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>coeff2_d</t>
+  </si>
+  <si>
+    <t>coeff1_d</t>
+  </si>
+  <si>
+    <t>coeff0_d</t>
+  </si>
+  <si>
+    <t>d_plus</t>
+  </si>
+  <si>
+    <t>d_minus</t>
+  </si>
+  <si>
+    <t>2 Practice</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>2 Real</t>
+  </si>
+  <si>
+    <t>4 Practice</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>up_pay</t>
+  </si>
+  <si>
+    <t>down_pay</t>
+  </si>
+  <si>
+    <t>disc_val</t>
+  </si>
+  <si>
+    <t>4 Real</t>
+  </si>
+  <si>
+    <t>S_0</t>
+  </si>
+  <si>
+    <t>up_down</t>
+  </si>
+  <si>
+    <t>payoff</t>
+  </si>
+  <si>
+    <t>5 Practice</t>
+  </si>
+  <si>
+    <t>eq</t>
+  </si>
+  <si>
+    <t>strike</t>
+  </si>
+  <si>
+    <t>d^2</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>numer</t>
+  </si>
+  <si>
+    <t>denom</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>1_over_g^2</t>
+  </si>
+  <si>
+    <t>1_less_p^2</t>
+  </si>
+  <si>
+    <t>val_check</t>
+  </si>
+  <si>
+    <t>5 Real</t>
+  </si>
+  <si>
+    <t>u^2</t>
   </si>
 </sst>
 </file>
@@ -70,13 +230,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -102,6 +270,53 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table911" displayName="Table911" ref="A30:P31" totalsRowShown="0">
+  <autoFilter ref="A30:P31"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="up"/>
+    <tableColumn id="2" name="down"/>
+    <tableColumn id="3" name="eq"/>
+    <tableColumn id="4" name="val"/>
+    <tableColumn id="5" name="strike"/>
+    <tableColumn id="6" name="up_down">
+      <calculatedColumnFormula>$A31*$B31*$C31</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="u^2">
+      <calculatedColumnFormula>$A31*$A31*$C31</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="payoff">
+      <calculatedColumnFormula>-$E31+$G31</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="root">
+      <calculatedColumnFormula>SQRT($D31/$H31)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="numer">
+      <calculatedColumnFormula>$B31</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="denom">
+      <calculatedColumnFormula>1-$I31*$A31+$I31*$B31</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="g">
+      <calculatedColumnFormula>$J31/$K31</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" name="r">
+      <calculatedColumnFormula>$L31-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="p">
+      <calculatedColumnFormula>($L31-$B31)/($A31-$B31)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" name="val_check">
+      <calculatedColumnFormula>$H31*$N31*$N31/($L31*$L31)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" name="answer">
+      <calculatedColumnFormula>1/$L31</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:B5" totalsRowShown="0">
   <autoFilter ref="A4:B5"/>
@@ -112,6 +327,236 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:N3" totalsRowShown="0">
+  <autoFilter ref="A2:N3"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="ret"/>
+    <tableColumn id="2" name="var"/>
+    <tableColumn id="3" name="down"/>
+    <tableColumn id="4" name="growth">
+      <calculatedColumnFormula>1+$A3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="coeff2_u">
+      <calculatedColumnFormula>$D3-$C3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="coeff1_u">
+      <calculatedColumnFormula>$C3*$C3-$D3*$D3-$B3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="coeff0_u">
+      <calculatedColumnFormula>-$D3*$C3*$C3+$D3*$D3*$C3+$B3*$C3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="ncoeff1">
+      <calculatedColumnFormula>$F3/$E3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="ncoeff0">
+      <calculatedColumnFormula>$G3/$E3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="sqrt">
+      <calculatedColumnFormula>SQRT($H3*$H3/4-$I3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="const">
+      <calculatedColumnFormula>-$H3/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="u_plus">
+      <calculatedColumnFormula>$K3+$J3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" name="u_minus">
+      <calculatedColumnFormula>$K3-$J3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="p">
+      <calculatedColumnFormula>($D3-$C3)/($L3-$C3)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table13" displayName="Table13" ref="A6:N7" totalsRowShown="0">
+  <autoFilter ref="A6:N7"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="ret"/>
+    <tableColumn id="2" name="var"/>
+    <tableColumn id="3" name="up"/>
+    <tableColumn id="4" name="growth">
+      <calculatedColumnFormula>1+$A7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="coeff2_d">
+      <calculatedColumnFormula>$C7-$D7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="coeff1_d">
+      <calculatedColumnFormula>-$C7*$C7+$D7*$D7+$B7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="coeff0_d">
+      <calculatedColumnFormula>$D7*$C7*$C7-$D7*$D7*$C7-$B7*$C7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="ncoeff1">
+      <calculatedColumnFormula>$F7/$E7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="ncoeff0">
+      <calculatedColumnFormula>$G7/$E7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="sqrt">
+      <calculatedColumnFormula>SQRT($H7*$H7/4-$I7)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="const">
+      <calculatedColumnFormula>-$H7/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="d_plus">
+      <calculatedColumnFormula>$K7+$J7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" name="d_minus">
+      <calculatedColumnFormula>$K7-$J7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="p">
+      <calculatedColumnFormula>($D7-$M7)/($C7-$M7)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A10:F11" totalsRowShown="0">
+  <autoFilter ref="A10:F11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="b"/>
+    <tableColumn id="2" name="r"/>
+    <tableColumn id="3" name="stock"/>
+    <tableColumn id="4" name="g">
+      <calculatedColumnFormula>1+$B11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="a">
+      <calculatedColumnFormula>-$A11*$C11/$D11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="cost">
+      <calculatedColumnFormula>$A11*$C11+$E11</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="A14:F15" totalsRowShown="0">
+  <autoFilter ref="A14:F15"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="b"/>
+    <tableColumn id="2" name="r"/>
+    <tableColumn id="3" name="stock"/>
+    <tableColumn id="4" name="g">
+      <calculatedColumnFormula>1+$B15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="a">
+      <calculatedColumnFormula>-$A15*$C15/$D15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="cost">
+      <calculatedColumnFormula>$A15*$C15+$E15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A18:H19" totalsRowShown="0">
+  <autoFilter ref="A18:H19"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="rate"/>
+    <tableColumn id="2" name="up"/>
+    <tableColumn id="3" name="down"/>
+    <tableColumn id="4" name="q" dataDxfId="1">
+      <calculatedColumnFormula>(1+$A19-$C19)/($B19-$C19)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="up_pay"/>
+    <tableColumn id="6" name="down_pay"/>
+    <tableColumn id="7" name="val">
+      <calculatedColumnFormula>POWER($D19,5)*$E19+POWER(1-$D19,5)*$F19</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="disc_val">
+      <calculatedColumnFormula>$G19/POWER(1+$A19,5)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table79" displayName="Table79" ref="A22:I23" totalsRowShown="0">
+  <autoFilter ref="A22:I23"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="rate"/>
+    <tableColumn id="2" name="up"/>
+    <tableColumn id="3" name="down"/>
+    <tableColumn id="4" name="q" dataDxfId="0">
+      <calculatedColumnFormula>(1+$A23-$C23)/($B23-$C23)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="S_0"/>
+    <tableColumn id="6" name="up_down">
+      <calculatedColumnFormula>$B23*$C23*$E23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="payoff">
+      <calculatedColumnFormula>POWER($B23*$B23*$E23, 2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="val">
+      <calculatedColumnFormula>POWER($D23,2)*$G23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="disc_val">
+      <calculatedColumnFormula>$H23/POWER(1+$A23,2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A26:P27" totalsRowShown="0">
+  <autoFilter ref="A26:P27"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="up"/>
+    <tableColumn id="2" name="down"/>
+    <tableColumn id="3" name="eq"/>
+    <tableColumn id="4" name="val"/>
+    <tableColumn id="5" name="strike"/>
+    <tableColumn id="6" name="up_down">
+      <calculatedColumnFormula>$A27*$B27*$C27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="d^2">
+      <calculatedColumnFormula>$B27*$B27*$C27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="payoff">
+      <calculatedColumnFormula>$E27-$G27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="root">
+      <calculatedColumnFormula>SQRT($D27/$H27)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="numer">
+      <calculatedColumnFormula>$A27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="denom">
+      <calculatedColumnFormula>1+$I27*$A27-$I27*$B27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="g">
+      <calculatedColumnFormula>$J27/$K27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" name="r">
+      <calculatedColumnFormula>$L27-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="1_over_g^2">
+      <calculatedColumnFormula>1/($L27*$L27)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" name="1_less_p^2">
+      <calculatedColumnFormula>($A27-$L27)/($A27-$B27)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" name="val_check">
+      <calculatedColumnFormula>$H27*$N27*$O27*$O27</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -380,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F1:P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -436,4 +881,700 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M19" sqref="M18:M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="7" width="10.36328125" customWidth="1"/>
+    <col min="8" max="9" width="9.36328125" customWidth="1"/>
+    <col min="13" max="13" width="9.36328125" customWidth="1"/>
+    <col min="14" max="15" width="12.36328125" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.01</v>
+      </c>
+      <c r="B3">
+        <v>1.89E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.8</v>
+      </c>
+      <c r="D3">
+        <f>1+$A3</f>
+        <v>1.01</v>
+      </c>
+      <c r="E3">
+        <f>$D3-$C3</f>
+        <v>0.20999999999999996</v>
+      </c>
+      <c r="F3">
+        <f>$C3*$C3-$D3*$D3-$B3</f>
+        <v>-0.39899999999999991</v>
+      </c>
+      <c r="G3">
+        <f>-$D3*$C3*$C3+$D3*$D3*$C3+$B3*$C3</f>
+        <v>0.18479999999999994</v>
+      </c>
+      <c r="H3">
+        <f>$F3/$E3</f>
+        <v>-1.9</v>
+      </c>
+      <c r="I3">
+        <f>$G3/$E3</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="J3">
+        <f>SQRT($H3*$H3/4-$I3)</f>
+        <v>0.15000000000000024</v>
+      </c>
+      <c r="K3">
+        <f>-$H3/2</f>
+        <v>0.95</v>
+      </c>
+      <c r="L3">
+        <f>$K3+$J3</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M3">
+        <f>$K3-$J3</f>
+        <v>0.79999999999999971</v>
+      </c>
+      <c r="N3">
+        <f>($D3-$C3)/($L3-$C3)</f>
+        <v>0.69999999999999973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.02</v>
+      </c>
+      <c r="B7">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="C7">
+        <v>1.2</v>
+      </c>
+      <c r="D7">
+        <f>1+$A7</f>
+        <v>1.02</v>
+      </c>
+      <c r="E7">
+        <f>$C7-$D7</f>
+        <v>0.17999999999999994</v>
+      </c>
+      <c r="F7">
+        <f>-$C7*$C7+$D7*$D7+$B7</f>
+        <v>-0.37799999999999995</v>
+      </c>
+      <c r="G7">
+        <f>$D7*$C7*$C7-$D7*$D7*$C7-$B7*$C7</f>
+        <v>0.19439999999999985</v>
+      </c>
+      <c r="H7">
+        <f>$F7/$E7</f>
+        <v>-2.1000000000000005</v>
+      </c>
+      <c r="I7">
+        <f>$G7/$E7</f>
+        <v>1.0799999999999996</v>
+      </c>
+      <c r="J7">
+        <f>SQRT($H7*$H7/4-$I7)</f>
+        <v>0.15000000000000285</v>
+      </c>
+      <c r="K7">
+        <f>-$H7/2</f>
+        <v>1.0500000000000003</v>
+      </c>
+      <c r="L7">
+        <f>$K7+$J7</f>
+        <v>1.2000000000000031</v>
+      </c>
+      <c r="M7">
+        <f>$K7-$J7</f>
+        <v>0.89999999999999747</v>
+      </c>
+      <c r="N7">
+        <f>($D7-$M7)/($C7-$M7)</f>
+        <v>0.40000000000000518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>-0.5</v>
+      </c>
+      <c r="B11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <f>1+$B11</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="E11">
+        <f>-$A11*$C11/$D11</f>
+        <v>49.75124378109453</v>
+      </c>
+      <c r="F11">
+        <f>$A11*$C11+$E11</f>
+        <v>-0.24875621890546995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0.01</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <f>1+$B15</f>
+        <v>1.01</v>
+      </c>
+      <c r="E15">
+        <f>-$A15*$C15/$D15</f>
+        <v>-99.009900990099013</v>
+      </c>
+      <c r="F15">
+        <f>$A15*$C15+$E15</f>
+        <v>0.99009900990098743</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.05</v>
+      </c>
+      <c r="B19">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C19">
+        <v>0.92</v>
+      </c>
+      <c r="D19" s="1">
+        <f>(1+$A19-$C19)/($B19-$C19)</f>
+        <v>0.6499999999999998</v>
+      </c>
+      <c r="E19">
+        <v>40</v>
+      </c>
+      <c r="F19">
+        <v>1000</v>
+      </c>
+      <c r="G19">
+        <f>POWER($D19,5)*$E19+POWER(1-$D19,5)*$F19</f>
+        <v>9.8933500000000087</v>
+      </c>
+      <c r="H19">
+        <f>$G19/POWER(1+$A19,5)</f>
+        <v>7.7516985990307354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0.01</v>
+      </c>
+      <c r="B23">
+        <v>1.02</v>
+      </c>
+      <c r="C23">
+        <v>0.98</v>
+      </c>
+      <c r="D23" s="1">
+        <f>(1+$A23-$C23)/($B23-$C23)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <f>$B23*$C23*$E23</f>
+        <v>99.960000000000008</v>
+      </c>
+      <c r="G23">
+        <f>POWER($B23*$B23*$E23, 2)</f>
+        <v>10824.321599999997</v>
+      </c>
+      <c r="H23">
+        <f>POWER($D23,2)*$G23</f>
+        <v>6088.6808999999985</v>
+      </c>
+      <c r="I23">
+        <f>$H23/POWER(1+$A23,2)</f>
+        <v>5968.7098323693745</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K26" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" t="s">
+        <v>52</v>
+      </c>
+      <c r="O26" t="s">
+        <v>53</v>
+      </c>
+      <c r="P26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B27">
+        <v>0.95</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>0.44153700000000001</v>
+      </c>
+      <c r="E27">
+        <v>94</v>
+      </c>
+      <c r="F27">
+        <f>$A27*$B27*$C27</f>
+        <v>109.24999999999999</v>
+      </c>
+      <c r="G27">
+        <f>$B27*$B27*$C27</f>
+        <v>90.25</v>
+      </c>
+      <c r="H27">
+        <f>$E27-$G27</f>
+        <v>3.75</v>
+      </c>
+      <c r="I27">
+        <f>SQRT($D27/$H27)</f>
+        <v>0.34313729030812146</v>
+      </c>
+      <c r="J27">
+        <f>$A27</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K27">
+        <f>1+$I27*$A27-$I27*$B27</f>
+        <v>1.0686274580616244</v>
+      </c>
+      <c r="L27">
+        <f>$J27/$K27</f>
+        <v>1.0761467818597668</v>
+      </c>
+      <c r="M27">
+        <f>$L27-1</f>
+        <v>7.6146781859766755E-2</v>
+      </c>
+      <c r="N27">
+        <f>1/($L27*$L27)</f>
+        <v>0.86348933393062288</v>
+      </c>
+      <c r="O27">
+        <f>($A27-$L27)/($A27-$B27)</f>
+        <v>0.36926609070116584</v>
+      </c>
+      <c r="P27">
+        <f>$H27*$N27*$O27*$O27</f>
+        <v>0.44153700000000101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" t="s">
+        <v>49</v>
+      </c>
+      <c r="K30" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" t="s">
+        <v>18</v>
+      </c>
+      <c r="O30" t="s">
+        <v>54</v>
+      </c>
+      <c r="P30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B31">
+        <v>0.95</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
+      </c>
+      <c r="D31">
+        <v>5.4240000000000004</v>
+      </c>
+      <c r="E31">
+        <v>115</v>
+      </c>
+      <c r="F31">
+        <f>$A31*$B31*$C31</f>
+        <v>109.24999999999999</v>
+      </c>
+      <c r="G31">
+        <f>$A31*$A31*$C31</f>
+        <v>132.24999999999997</v>
+      </c>
+      <c r="H31">
+        <f>-$E31+$G31</f>
+        <v>17.249999999999972</v>
+      </c>
+      <c r="I31">
+        <f>SQRT($D31/$H31)</f>
+        <v>0.56074484626137777</v>
+      </c>
+      <c r="J31">
+        <f>$B31</f>
+        <v>0.95</v>
+      </c>
+      <c r="K31">
+        <f>1-$I31*$A31+$I31*$B31</f>
+        <v>0.88785103074772442</v>
+      </c>
+      <c r="L31">
+        <f>$J31/$K31</f>
+        <v>1.069999320944568</v>
+      </c>
+      <c r="M31">
+        <f>$L31-1</f>
+        <v>6.9999320944567955E-2</v>
+      </c>
+      <c r="N31">
+        <f>($L31-$B31)/($A31-$B31)</f>
+        <v>0.59999660472284011</v>
+      </c>
+      <c r="O31">
+        <f>$H31*$N31*$N31/($L31*$L31)</f>
+        <v>5.4239999999999959</v>
+      </c>
+      <c r="P31">
+        <f>1/$L31</f>
+        <v>0.93458003236602583</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="8">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>